<commit_message>
add form and importer and pass test
</commit_message>
<xml_diff>
--- a/src/templates/ChargeTableTemplate.xlsx
+++ b/src/templates/ChargeTableTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\php\yii2exts\exts\48-yii2-charging\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5988EC8-B64B-4F88-97B1-FE88F5B81018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EC4C96-51AA-4658-B575-1989746EC550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27885" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>ChargeType</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,10 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>仓储费</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CMB/Day</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -74,23 +70,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>出库费</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>入库费</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>KG</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>入库费出库时收</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DiscountPercent(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemStorage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OutboundHandling</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -475,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -529,12 +521,12 @@
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -543,19 +535,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3">
         <v>31</v>
@@ -564,19 +556,19 @@
         <v>60</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3">
         <v>0.35</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3">
         <v>61</v>
@@ -585,61 +577,61 @@
         <v>999</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3">
         <v>0.6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3">
-        <v>0.17</v>
+        <v>0.06</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3">
-        <v>0.24</v>
+        <v>0.17</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -648,222 +640,87 @@
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3">
-        <v>0.62</v>
+        <v>0.17</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
       </c>
       <c r="H7" s="3">
-        <v>0.09</v>
-      </c>
-      <c r="K7" s="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="I7" s="3">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3">
+        <v>20</v>
+      </c>
+      <c r="K7" s="3">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E8" s="3">
-        <v>0.05</v>
+        <v>0.17</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="I8" s="3">
+        <v>20</v>
+      </c>
+      <c r="J8" s="3">
+        <v>30</v>
+      </c>
+      <c r="K8" s="3">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.06</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="F9" s="4"/>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.17</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="F10" s="4"/>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.17</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="I11" s="3">
-        <v>10</v>
-      </c>
-      <c r="J11" s="3">
-        <v>20</v>
-      </c>
-      <c r="K11" s="3">
-        <v>30</v>
-      </c>
+      <c r="F11" s="4"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.17</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="I12" s="3">
-        <v>20</v>
-      </c>
-      <c r="J12" s="3">
-        <v>30</v>
-      </c>
-      <c r="K12" s="3">
-        <v>40</v>
-      </c>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.17</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.24</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3">
-        <v>10</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.62</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0.09</v>
-      </c>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
@@ -907,18 +764,6 @@
     </row>
     <row r="29" spans="11:11" x14ac:dyDescent="0.15">
       <c r="K29" s="3"/>
-    </row>
-    <row r="30" spans="11:11" x14ac:dyDescent="0.15">
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="11:11" x14ac:dyDescent="0.15">
-      <c r="K31" s="3"/>
-    </row>
-    <row r="32" spans="11:11" x14ac:dyDescent="0.15">
-      <c r="K32" s="3"/>
-    </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.15">
-      <c r="K33" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>